<commit_message>
✨feature: 'Change pdf finops'
</commit_message>
<xml_diff>
--- a/docs/examples/files/bootcamp-devsecops.xlsx
+++ b/docs/examples/files/bootcamp-devsecops.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\aws-devsecops-migration\docs\examples\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5BBC7-1BBB-4263-92D1-3D8FC01A1C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB1A964-7B5F-4BA5-B260-3348565E69B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{6C97D93F-911F-4047-BB4B-AB449348E287}"/>
+    <workbookView xWindow="-38520" yWindow="-12555" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{6C97D93F-911F-4047-BB4B-AB449348E287}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bootcamp" sheetId="1" r:id="rId1"/>
-    <sheet name="DevSecOps" sheetId="2" r:id="rId2"/>
+    <sheet name="DevOps" sheetId="2" r:id="rId1"/>
+    <sheet name="Bootcamp" sheetId="1" r:id="rId2"/>
+    <sheet name="Paquetes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="142">
   <si>
     <t>Herramienta.</t>
   </si>
@@ -422,16 +423,80 @@
   <si>
     <t>SQS.</t>
   </si>
+  <si>
+    <t>Duración</t>
+  </si>
+  <si>
+    <t>Días incluidos</t>
+  </si>
+  <si>
+    <t>Precio final (COP)</t>
+  </si>
+  <si>
+    <t>1 día</t>
+  </si>
+  <si>
+    <t>$2,300,000</t>
+  </si>
+  <si>
+    <t>$0</t>
+  </si>
+  <si>
+    <t>1 semana</t>
+  </si>
+  <si>
+    <t>$16,100,000</t>
+  </si>
+  <si>
+    <t>$7,000,000</t>
+  </si>
+  <si>
+    <t>$9,100,000</t>
+  </si>
+  <si>
+    <t>2 semanas</t>
+  </si>
+  <si>
+    <t>$32,200,000</t>
+  </si>
+  <si>
+    <t>$16,000,000</t>
+  </si>
+  <si>
+    <t>$16,200,000</t>
+  </si>
+  <si>
+    <t>4 semanas</t>
+  </si>
+  <si>
+    <t>$64,400,000</t>
+  </si>
+  <si>
+    <t>$44,000,000</t>
+  </si>
+  <si>
+    <t>$20,400,000</t>
+  </si>
+  <si>
+    <t>Ahorro</t>
+  </si>
+  <si>
+    <t>Descuento aplicado</t>
+  </si>
+  <si>
+    <t>Precio total sin descuento</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$$-240A]\ #,##0.0000"/>
-    <numFmt numFmtId="168" formatCode="[$$-240A]\ #,##0.00"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$$-240A]\ #,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="[$$-240A]\ #,##0.00"/>
+    <numFmt numFmtId="170" formatCode="[$$-240A]\ #,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,8 +542,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,6 +631,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -686,6 +781,73 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -704,25 +866,22 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -737,68 +896,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1114,13 +1230,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED7267F-BF50-41DB-8809-392E606FB54C}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="55"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="53"/>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9BDB49-9AC7-40EA-8B0C-2E0583636109}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -1133,8 +1360,8 @@
     <col min="5" max="5" width="21.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" style="52" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="52"/>
+    <col min="8" max="8" width="7" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="24"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="44.85546875" customWidth="1"/>
@@ -1166,13 +1393,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="A2" s="40">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="40" t="s">
         <v>81</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -1181,31 +1408,31 @@
       <c r="E2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="17">
         <v>0</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="18">
         <v>0</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="7" t="s">
         <v>43</v>
       </c>
@@ -1213,16 +1440,16 @@
         <v>112</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="38">
+      <c r="F4" s="18">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="41"/>
+      <c r="B5" s="43" t="s">
         <v>69</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -1234,14 +1461,14 @@
       <c r="E5" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="19">
         <v>0</v>
       </c>
-      <c r="G5" s="19"/>
+      <c r="G5" s="42"/>
     </row>
     <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="9" t="s">
         <v>77</v>
       </c>
@@ -1251,16 +1478,16 @@
       <c r="E6" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="19">
         <v>1</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="21"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="9" t="s">
         <v>78</v>
       </c>
@@ -1268,77 +1495,77 @@
         <v>39</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="F7" s="39">
+      <c r="F7" s="19">
         <v>0</v>
       </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="45"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="20" t="s">
+      <c r="A8" s="41"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="43" t="s">
         <v>116</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>80</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="39">
+      <c r="F8" s="19">
         <v>1</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="41"/>
+      <c r="B9" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="39">
+      <c r="F9" s="19">
         <v>0</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="45"/>
     </row>
     <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="47">
         <v>0</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="19"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="42"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="17" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="40" t="s">
         <v>74</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1347,45 +1574,45 @@
       <c r="E12" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="18">
         <v>0</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="38">
+      <c r="F13" s="18">
         <f>0.25*2</f>
         <v>0.5</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="8"/>
-      <c r="F14" s="38">
+      <c r="F14" s="18">
         <v>3.3330000000000002</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="41"/>
+      <c r="B15" s="43" t="s">
         <v>57</v>
       </c>
       <c r="C15" s="10"/>
@@ -1393,29 +1620,29 @@
         <v>52</v>
       </c>
       <c r="E15" s="11"/>
-      <c r="F15" s="42">
+      <c r="F15" s="20">
         <v>0.15</v>
       </c>
-      <c r="G15" s="22"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="42">
+      <c r="F16" s="20">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="41"/>
+      <c r="B17" s="40" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1425,19 +1652,19 @@
         <v>51</v>
       </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="38">
+      <c r="F17" s="18">
         <f>H17*G16</f>
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="52">
+      <c r="G17" s="45"/>
+      <c r="H17" s="24">
         <f>0.0225+0.008</f>
         <v>3.0499999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="7" t="s">
         <v>63</v>
       </c>
@@ -1447,16 +1674,16 @@
       <c r="E18" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="17">
         <v>0</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="7" t="s">
         <v>97</v>
       </c>
@@ -1466,14 +1693,14 @@
       <c r="E19" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F19" s="37">
+      <c r="F19" s="17">
         <v>3.3332999999999999</v>
       </c>
-      <c r="G19" s="19"/>
+      <c r="G19" s="42"/>
     </row>
     <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="7" t="s">
         <v>100</v>
       </c>
@@ -1481,17 +1708,17 @@
         <v>99</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="37">
+      <c r="F20" s="17">
         <f>0.05*2</f>
         <v>0.1</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="7" t="s">
         <v>102</v>
       </c>
@@ -1499,73 +1726,73 @@
         <v>101</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="37">
+      <c r="F21" s="17">
         <v>0</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="42"/>
     </row>
     <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="42"/>
       <c r="C22" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="49">
         <f>0.1*2</f>
         <v>0.2</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="20" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="43" t="s">
         <v>118</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="22"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="45"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="21"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="20">
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="22"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="45"/>
     </row>
     <row r="26" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
+      <c r="A26" s="31">
         <v>2</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="32" t="s">
         <v>66</v>
       </c>
       <c r="C26" s="12" t="s">
@@ -1575,16 +1802,16 @@
         <v>103</v>
       </c>
       <c r="E26" s="13"/>
-      <c r="F26" s="46">
+      <c r="F26" s="21">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G26" s="35">
+      <c r="G26" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="13" t="s">
         <v>105</v>
       </c>
@@ -1592,14 +1819,14 @@
         <v>104</v>
       </c>
       <c r="E27" s="13"/>
-      <c r="F27" s="46">
+      <c r="F27" s="21">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G27" s="35"/>
+      <c r="G27" s="30"/>
     </row>
     <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="24"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="13" t="s">
         <v>49</v>
       </c>
@@ -1607,16 +1834,16 @@
         <v>107</v>
       </c>
       <c r="E28" s="13"/>
-      <c r="F28" s="46">
+      <c r="F28" s="21">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G28" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="24"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="13" t="s">
         <v>55</v>
       </c>
@@ -1626,15 +1853,15 @@
       <c r="E29" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="47">
+      <c r="F29" s="22">
         <f>0.1866+0.0001</f>
         <v>0.18669999999999998</v>
       </c>
-      <c r="G29" s="35"/>
+      <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="13" t="s">
         <v>43</v>
       </c>
@@ -1642,16 +1869,16 @@
         <v>40</v>
       </c>
       <c r="E30" s="13"/>
-      <c r="F30" s="46">
+      <c r="F30" s="21">
         <v>0</v>
       </c>
-      <c r="G30" s="29">
+      <c r="G30" s="31">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="26" t="s">
+      <c r="A31" s="31"/>
+      <c r="B31" s="46" t="s">
         <v>73</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -1661,14 +1888,14 @@
         <v>108</v>
       </c>
       <c r="E31" s="13"/>
-      <c r="F31" s="46">
+      <c r="F31" s="21">
         <v>1.66E-2</v>
       </c>
-      <c r="G31" s="29"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="14" t="s">
         <v>47</v>
       </c>
@@ -1676,16 +1903,16 @@
         <v>41</v>
       </c>
       <c r="E32" s="14"/>
-      <c r="F32" s="48">
+      <c r="F32" s="23">
         <v>0</v>
       </c>
-      <c r="G32" s="35">
+      <c r="G32" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="14" t="s">
         <v>110</v>
       </c>
@@ -1693,14 +1920,14 @@
         <v>119</v>
       </c>
       <c r="E33" s="14"/>
-      <c r="F33" s="48">
+      <c r="F33" s="23">
         <v>0</v>
       </c>
-      <c r="G33" s="35"/>
+      <c r="G33" s="30"/>
     </row>
     <row r="34" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="14" t="s">
         <v>111</v>
       </c>
@@ -1708,57 +1935,57 @@
         <v>120</v>
       </c>
       <c r="E34" s="14"/>
-      <c r="F34" s="48">
+      <c r="F34" s="23">
         <v>0</v>
       </c>
-      <c r="G34" s="35">
+      <c r="G34" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="24" t="s">
+      <c r="A35" s="31"/>
+      <c r="B35" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="33" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E35" s="13"/>
-      <c r="F35" s="46">
+      <c r="F35" s="21">
         <v>0</v>
       </c>
-      <c r="G35" s="35"/>
+      <c r="G35" s="30"/>
     </row>
     <row r="36" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
       <c r="D36" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="13"/>
-      <c r="F36" s="46">
+      <c r="F36" s="21">
         <f>H36+I36</f>
         <v>0.34329999999999999</v>
       </c>
-      <c r="G36" s="35">
+      <c r="G36" s="30">
         <v>2</v>
       </c>
-      <c r="H36" s="52">
+      <c r="H36" s="24">
         <f>0.3333</f>
         <v>0.33329999999999999</v>
       </c>
-      <c r="I36" s="52">
+      <c r="I36" s="24">
         <f>0.005*2</f>
         <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="13" t="s">
         <v>45</v>
       </c>
@@ -1766,59 +1993,59 @@
         <v>28</v>
       </c>
       <c r="E37" s="13"/>
-      <c r="F37" s="46">
+      <c r="F37" s="21">
         <v>0</v>
       </c>
-      <c r="G37" s="35"/>
+      <c r="G37" s="30"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="23" t="s">
+      <c r="A38" s="31"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="32" t="s">
         <v>46</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>38</v>
       </c>
       <c r="E38" s="13"/>
-      <c r="F38" s="46">
+      <c r="F38" s="21">
         <v>0</v>
       </c>
-      <c r="G38" s="35">
+      <c r="G38" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E39" s="13"/>
-      <c r="F39" s="46">
+      <c r="F39" s="21">
         <v>0</v>
       </c>
-      <c r="G39" s="35"/>
+      <c r="G39" s="30"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
       <c r="D40" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E40" s="13"/>
-      <c r="F40" s="46">
+      <c r="F40" s="21">
         <v>0</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40" s="31">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="27" t="s">
+      <c r="A41" s="31"/>
+      <c r="B41" s="38" t="s">
         <v>67</v>
       </c>
       <c r="C41" s="15" t="s">
@@ -1828,108 +2055,144 @@
         <v>35</v>
       </c>
       <c r="E41" s="14"/>
-      <c r="F41" s="48">
+      <c r="F41" s="23">
         <v>1</v>
       </c>
-      <c r="G41" s="29"/>
+      <c r="G41" s="31"/>
     </row>
     <row r="42" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="49">
+      <c r="E42" s="32"/>
+      <c r="F42" s="35">
         <v>0</v>
       </c>
-      <c r="G42" s="35">
+      <c r="G42" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="23" t="s">
+      <c r="A43" s="31"/>
+      <c r="B43" s="32" t="s">
         <v>113</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="35"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="30"/>
     </row>
     <row r="44" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="35">
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="31"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="35"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="30"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="55">
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="27">
         <f>SUM(F$2:$F45)</f>
         <v>11.255199999999999</v>
       </c>
-      <c r="G46" s="36">
+      <c r="G46" s="29">
         <f>SUM($G$2:$G45)</f>
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="53">
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="25">
         <f>F46*G46</f>
         <v>495.22879999999992</v>
       </c>
-      <c r="G47" s="36"/>
+      <c r="G47" s="29"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="54">
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="26">
         <f>F47*11</f>
         <v>5447.5167999999994</v>
       </c>
-      <c r="G48" s="36"/>
+      <c r="G48" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="A26:A45"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="A46:E48"/>
     <mergeCell ref="G46:G48"/>
     <mergeCell ref="G42:G43"/>
@@ -1945,155 +2208,135 @@
     <mergeCell ref="F42:F45"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="E42:E45"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="A26:A45"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G24:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED7267F-BF50-41DB-8809-392E606FB54C}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49F281F-F9E7-4997-8DBC-D26FCBC9D00A}">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="57"/>
+    <col min="2" max="2" width="13.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="33"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="1">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
+      <c r="C4" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="1">
+        <v>24</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>